<commit_message>
edits in upload timesheet
</commit_message>
<xml_diff>
--- a/excelforms/الحصر - Copy.xlsx
+++ b/excelforms/الحصر - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lobna\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\payroll\excelforms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98B62F5-5874-46C1-83E7-CBD46AA9476C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED25BD74-5EEF-484B-A16B-0F70EFE5BB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="1185" windowWidth="18840" windowHeight="9180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,20 +405,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,7 +453,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1455</v>
       </c>
@@ -467,7 +467,7 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -482,7 +482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1100</v>
       </c>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1532</v>
       </c>

</xml_diff>

<commit_message>
edit in upload functions
</commit_message>
<xml_diff>
--- a/excelforms/الحصر - Copy.xlsx
+++ b/excelforms/الحصر - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\payroll\excelforms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED25BD74-5EEF-484B-A16B-0F70EFE5BB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7949349-161C-4F8E-B2E0-CF372FA0AF17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -406,19 +406,19 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -453,9 +453,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1455</v>
+        <v>1152</v>
       </c>
       <c r="C2">
         <v>30</v>
@@ -482,9 +482,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1100</v>
+        <v>167</v>
       </c>
       <c r="C3">
         <v>30</v>
@@ -511,9 +511,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1532</v>
+        <v>900</v>
       </c>
       <c r="C4">
         <v>30</v>
@@ -531,7 +531,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -542,8 +542,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>